<commit_message>
Update sets of the uncertainty table for testing
</commit_message>
<xml_diff>
--- a/src/Interface_RDM.xlsx
+++ b/src/Interface_RDM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\CCG_RDM\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9883719-64C7-4DD7-9651-73DD60BF814C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407ABC31-B397-478C-897B-BFAA091BB21A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="727" activeTab="1" xr2:uid="{A38498C0-325E-4D75-9B65-6D8B75ECDFF0}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="Params_Sets_Vari" sheetId="14" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Uncertainty_Table!$A$1:$N$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Uncertainty_Table!$A$1:$N$35</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="197">
   <si>
     <t>X_Num</t>
   </si>
@@ -546,42 +546,27 @@
     <t>Capital Cost of competing technologies</t>
   </si>
   <si>
-    <t xml:space="preserve"> RSA_POW_PP_HYDR ; RSA_POW_PP_CSP ; RSA_POW_PP_PV_UT ; RSA_POW_PP_PV_DIST ; RSA_POW_PP_WIND ; RSA_POW_STO_BAT_OUT ; RSA_POW_STO_PHY_OUT</t>
-  </si>
-  <si>
     <t>Fixed Cost</t>
   </si>
   <si>
     <t>Fixed Cost of competing technologies</t>
   </si>
   <si>
-    <t xml:space="preserve"> RSA_POW_PP_HYDR ; RSA_POW_PP_CSP ; RSA_POW_PP_PV_UT ; RSA_POW_PP_PV_DIST ; RSA_POW_PP_WIND </t>
-  </si>
-  <si>
     <t>Variable Cost</t>
   </si>
   <si>
     <t>Variable Cost of competing technologies</t>
   </si>
   <si>
-    <t xml:space="preserve"> RSA_POW_PP_HYDR ; RSA_POW_PP_CSP ; RSA_FUEL_PRO_NG  </t>
-  </si>
-  <si>
     <t>Capital Cost of competing technologies  FOSSIL</t>
   </si>
   <si>
-    <t xml:space="preserve">RSA_POW_PP_COAL ; RSA_POW_PP_MMG ; RSA_POW_PP_PEAK </t>
-  </si>
-  <si>
     <t>Fixed Cost of competing technologies   FOSSIL</t>
   </si>
   <si>
     <t>Variable Cost of competing technologies   FOSSIL</t>
   </si>
   <si>
-    <t>RSA_FUEL_PRO_COAL ; RSA_POW_PP_COAL ; RSA_POW_PP_MMG ; RSA_POW_PP_PEAK ; RSA_FUEL_PRO_DSL</t>
-  </si>
-  <si>
     <t>DiscountRateIdv</t>
   </si>
   <si>
@@ -621,27 +606,12 @@
     <t>Minimum non-intermittent capacity  the system should have</t>
   </si>
   <si>
-    <t>RSA_POW_TD</t>
-  </si>
-  <si>
     <t>Cost of Transimission grids</t>
   </si>
   <si>
     <t>Variable cost of interconnectors Export  Import</t>
   </si>
   <si>
-    <t>RSA_POW_INT</t>
-  </si>
-  <si>
-    <t>RSA_POW_PP_NU_OLD ; RSA_POW_PP_NU ; RSA_POW_PP_NU_SMR</t>
-  </si>
-  <si>
-    <t>MINLFSMR</t>
-  </si>
-  <si>
-    <t>RSA_POW_PP_NU_SMR</t>
-  </si>
-  <si>
     <t>Activity Upper Limit</t>
   </si>
   <si>
@@ -657,9 +627,6 @@
     <t>Change_Curve</t>
   </si>
   <si>
-    <t>RSA_POW_ELEF</t>
-  </si>
-  <si>
     <t>1) Select a curve from "shape_of_demand.xlsx". 2) The curve of the selected timeslices in the column “CF_timeslices” is changed to the selected curve of “shape_of_demand.xlsx”.</t>
   </si>
   <si>
@@ -711,54 +678,30 @@
     <t>Involved_First_Sets_in_Osemosys</t>
   </si>
   <si>
-    <t>1 ; 2</t>
-  </si>
-  <si>
     <t>Capital Cost Storage</t>
   </si>
   <si>
     <t>Capital Cost of competing technologies  storage</t>
   </si>
   <si>
-    <t>RSA_POW_STO_BAT ; RSA_POW_STO_PHY</t>
-  </si>
-  <si>
     <t>Capacity Factor</t>
   </si>
   <si>
-    <t>RSA_POW_PP_HYDR</t>
-  </si>
-  <si>
     <t>Activity Ratio of Inputs</t>
   </si>
   <si>
     <t>Factor of Capacities</t>
   </si>
   <si>
-    <t>RSA_POW_PP_COAL ; RSA_POW_PP_MMG</t>
-  </si>
-  <si>
-    <t>RSA_FUEL_COAL ; RSA_POW_H2</t>
-  </si>
-  <si>
     <t>Input Activity Ratio</t>
   </si>
   <si>
-    <t>Emission Penalty</t>
-  </si>
-  <si>
     <t>Penalty to Emissions</t>
   </si>
   <si>
-    <t>RSA_CO2</t>
-  </si>
-  <si>
     <t>Emission Activity Ratio</t>
   </si>
   <si>
-    <t>RSA_FUEL_PRO_COAL</t>
-  </si>
-  <si>
     <t>Constant</t>
   </si>
   <si>
@@ -771,19 +714,73 @@
     <t>Linear</t>
   </si>
   <si>
-    <t>All</t>
-  </si>
-  <si>
     <t>ALL</t>
   </si>
   <si>
     <t>cplex</t>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>model.v.5.3.txt</t>
+  </si>
+  <si>
+    <t>AGRGSLMCH ; AGRDSLMCH</t>
+  </si>
+  <si>
+    <t>TRADSLPRL ; TRAELCPRL</t>
+  </si>
+  <si>
+    <t>INDOTHELCHTH ; INDOTHDSLHTH</t>
+  </si>
+  <si>
+    <t>DEMINDHDG ; DEMINDCOA</t>
+  </si>
+  <si>
+    <t>LVSCTLIMP ; LVSSHPIMP</t>
+  </si>
+  <si>
+    <t>RESELCCKNR</t>
+  </si>
+  <si>
+    <t>TRAEVSCHG001 ; TRAEVSCHG002</t>
+  </si>
+  <si>
+    <t>INDOTHELCHTH</t>
+  </si>
+  <si>
+    <t>AGRDSLMCH ; AGRGSLMCH</t>
+  </si>
+  <si>
+    <t>STGBAT</t>
+  </si>
+  <si>
+    <t>RESELCCKNU</t>
+  </si>
+  <si>
+    <t>RESELCCKGBALU</t>
+  </si>
+  <si>
+    <t>RESLPGCKNR</t>
+  </si>
+  <si>
+    <t>INDELC</t>
+  </si>
+  <si>
+    <t>RESELCCURR</t>
+  </si>
+  <si>
+    <t>S11 ; S12</t>
+  </si>
+  <si>
+    <t>LNDPET ; INDOTHELCHTH</t>
+  </si>
+  <si>
+    <t>LND ; INDELC</t>
+  </si>
+  <si>
+    <t>DEMINDWST</t>
+  </si>
+  <si>
+    <t>CO2</t>
   </si>
 </sst>
 </file>
@@ -1290,7 +1287,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1615,10 +1612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B5B787-8749-47D9-9D7A-FB53FE5A30D3}">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1671,13 +1668,13 @@
         <v>8</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="L1" s="54" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="M1" s="50" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="N1" s="33" t="s">
         <v>9</v>
@@ -1697,7 +1694,7 @@
         <v>22</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="F2" s="31" t="s">
         <v>10</v>
@@ -1715,7 +1712,7 @@
         <v>11</v>
       </c>
       <c r="K2" s="32" t="s">
-        <v>147</v>
+        <v>177</v>
       </c>
       <c r="L2" s="43" t="s">
         <v>12</v>
@@ -1741,7 +1738,7 @@
         <v>22</v>
       </c>
       <c r="E3" s="43" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="F3" s="43" t="s">
         <v>10</v>
@@ -1759,7 +1756,7 @@
         <v>11</v>
       </c>
       <c r="K3" s="44" t="s">
-        <v>118</v>
+        <v>178</v>
       </c>
       <c r="L3" s="43" t="s">
         <v>12</v>
@@ -1776,16 +1773,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="43" t="s">
+        <v>118</v>
+      </c>
+      <c r="C4" s="44" t="s">
         <v>119</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>120</v>
       </c>
       <c r="D4" s="43" t="s">
         <v>22</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="F4" s="43" t="s">
         <v>10</v>
@@ -1803,7 +1800,7 @@
         <v>14</v>
       </c>
       <c r="K4" s="44" t="s">
-        <v>121</v>
+        <v>179</v>
       </c>
       <c r="L4" s="43" t="s">
         <v>12</v>
@@ -1820,16 +1817,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="43" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D5" s="43" t="s">
         <v>22</v>
       </c>
       <c r="E5" s="43" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
       <c r="F5" s="43" t="s">
         <v>10</v>
@@ -1847,10 +1844,10 @@
         <v>15</v>
       </c>
       <c r="K5" s="44" t="s">
-        <v>124</v>
-      </c>
-      <c r="L5" s="55" t="s">
-        <v>173</v>
+        <v>180</v>
+      </c>
+      <c r="L5" s="55">
+        <v>1</v>
       </c>
       <c r="M5" s="43" t="s">
         <v>12</v>
@@ -1867,13 +1864,13 @@
         <v>23</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D6" s="43" t="s">
         <v>22</v>
       </c>
       <c r="E6" s="43" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="F6" s="43" t="s">
         <v>10</v>
@@ -1891,7 +1888,7 @@
         <v>11</v>
       </c>
       <c r="K6" s="44" t="s">
-        <v>126</v>
+        <v>183</v>
       </c>
       <c r="L6" s="43" t="s">
         <v>12</v>
@@ -1908,16 +1905,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D7" s="43" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="43" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
       <c r="F7" s="43" t="s">
         <v>10</v>
@@ -1935,7 +1932,7 @@
         <v>14</v>
       </c>
       <c r="K7" s="44" t="s">
-        <v>126</v>
+        <v>185</v>
       </c>
       <c r="L7" s="43" t="s">
         <v>12</v>
@@ -1952,16 +1949,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D8" s="31" t="s">
         <v>22</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="F8" s="31" t="s">
         <v>10</v>
@@ -1979,10 +1976,10 @@
         <v>15</v>
       </c>
       <c r="K8" s="32" t="s">
-        <v>129</v>
-      </c>
-      <c r="L8" s="43" t="s">
-        <v>173</v>
+        <v>181</v>
+      </c>
+      <c r="L8" s="55">
+        <v>1</v>
       </c>
       <c r="M8" s="43" t="s">
         <v>12</v>
@@ -1996,16 +1993,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>22</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="F9" s="31" t="s">
         <v>10</v>
@@ -2023,7 +2020,7 @@
         <v>36</v>
       </c>
       <c r="K9" s="32" t="s">
-        <v>176</v>
+        <v>186</v>
       </c>
       <c r="L9" s="43" t="s">
         <v>12</v>
@@ -2040,16 +2037,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="42" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D10" s="42" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="42" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="F10" s="42" t="s">
         <v>10</v>
@@ -2064,13 +2061,13 @@
         <v>1.2</v>
       </c>
       <c r="J10" s="42" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="K10" s="48" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="L10" s="42" t="s">
-        <v>148</v>
+        <v>188</v>
       </c>
       <c r="M10" s="42" t="s">
         <v>12</v>
@@ -2088,13 +2085,13 @@
         <v>23</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D11" s="20" t="s">
         <v>22</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>10</v>
@@ -2112,7 +2109,7 @@
         <v>11</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>143</v>
+        <v>184</v>
       </c>
       <c r="L11" s="51" t="s">
         <v>12</v>
@@ -2129,16 +2126,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>22</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>10</v>
@@ -2156,10 +2153,10 @@
         <v>15</v>
       </c>
       <c r="K12" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="L12" s="43" t="s">
-        <v>173</v>
+        <v>182</v>
+      </c>
+      <c r="L12" s="55">
+        <v>1</v>
       </c>
       <c r="M12" s="43" t="s">
         <v>12</v>
@@ -2173,16 +2170,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D13" s="15" t="s">
         <v>22</v>
       </c>
       <c r="E13" s="31" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="F13" s="15" t="s">
         <v>10</v>
@@ -2200,7 +2197,7 @@
         <v>68</v>
       </c>
       <c r="K13" s="32" t="s">
-        <v>146</v>
+        <v>189</v>
       </c>
       <c r="L13" s="40" t="s">
         <v>12</v>
@@ -2218,19 +2215,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D14" s="42" t="s">
         <v>22</v>
       </c>
       <c r="E14" s="42" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="F14" s="42" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="G14" s="42">
         <v>2036</v>
@@ -2245,16 +2242,16 @@
         <v>55</v>
       </c>
       <c r="K14" s="44" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="L14" s="40" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="M14" s="45" t="s">
         <v>12</v>
       </c>
       <c r="N14" s="46" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -2262,16 +2259,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>177</v>
+        <v>164</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
       <c r="D15" s="42" t="s">
         <v>22</v>
       </c>
       <c r="E15" s="42" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="F15" s="42" t="s">
         <v>10</v>
@@ -2289,16 +2286,16 @@
         <v>33</v>
       </c>
       <c r="K15" s="44" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="L15" s="40" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M15" s="45" t="s">
         <v>12</v>
       </c>
       <c r="N15" s="46" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:15" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -2306,16 +2303,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
       <c r="D16" s="42" t="s">
         <v>22</v>
       </c>
       <c r="E16" s="42" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="F16" s="42" t="s">
         <v>10</v>
@@ -2333,16 +2330,16 @@
         <v>46</v>
       </c>
       <c r="K16" s="44" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="L16" s="40" t="s">
-        <v>182</v>
-      </c>
-      <c r="M16" s="45" t="s">
-        <v>173</v>
+        <v>194</v>
+      </c>
+      <c r="M16" s="45">
+        <v>1</v>
       </c>
       <c r="N16" s="46" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:14" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -2350,22 +2347,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="D17" s="42" t="s">
         <v>22</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="F17" s="42" t="s">
         <v>10</v>
       </c>
       <c r="G17" s="42">
-        <v>2027</v>
+        <v>2023</v>
       </c>
       <c r="H17" s="43">
         <v>0.8</v>
@@ -2374,64 +2371,36 @@
         <v>1.2</v>
       </c>
       <c r="J17" s="40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K17" s="44" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="L17" s="40" t="s">
-        <v>12</v>
-      </c>
-      <c r="M17" s="45" t="s">
-        <v>12</v>
+        <v>196</v>
+      </c>
+      <c r="M17" s="45">
+        <v>1</v>
       </c>
       <c r="N17" s="46" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" s="1" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="39">
-        <v>17</v>
-      </c>
-      <c r="B18" s="40" t="s">
-        <v>187</v>
-      </c>
-      <c r="C18" s="41" t="s">
-        <v>185</v>
-      </c>
-      <c r="D18" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="42" t="s">
-        <v>190</v>
-      </c>
-      <c r="F18" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="G18" s="42">
-        <v>2023</v>
-      </c>
-      <c r="H18" s="43">
-        <v>0.8</v>
-      </c>
-      <c r="I18" s="43">
-        <v>1.2</v>
-      </c>
-      <c r="J18" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="K18" s="44" t="s">
-        <v>188</v>
-      </c>
-      <c r="L18" s="40" t="s">
-        <v>186</v>
-      </c>
-      <c r="M18" s="45" t="s">
-        <v>173</v>
-      </c>
-      <c r="N18" s="46" t="s">
-        <v>156</v>
-      </c>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="30"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="34"/>
     </row>
     <row r="19" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="30"/>
@@ -2705,23 +2674,8 @@
       <c r="M35" s="31"/>
       <c r="N35" s="34"/>
     </row>
-    <row r="36" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="30"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-      <c r="M36" s="31"/>
-      <c r="N36" s="34"/>
-    </row>
   </sheetData>
+  <autoFilter ref="A1:N35" xr:uid="{95B5B787-8749-47D9-9D7A-FB53FE5A30D3}"/>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2733,7 +2687,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2795,13 +2749,13 @@
         <v>27</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>196</v>
+        <v>27</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>197</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -3064,8 +3018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7095350F-2181-46D9-957F-C928CA3CEF59}">
   <dimension ref="A1:BG5"/>
   <sheetViews>
-    <sheetView topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AJ1" sqref="AJ1"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3129,7 +3083,7 @@
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="B1" t="s">
         <v>72</v>
@@ -3138,7 +3092,7 @@
         <v>43</v>
       </c>
       <c r="D1" s="52" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="E1" s="52" t="s">
         <v>71</v>
@@ -3174,7 +3128,7 @@
         <v>35</v>
       </c>
       <c r="P1" s="52" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="Q1" t="s">
         <v>34</v>
@@ -3195,16 +3149,16 @@
         <v>46</v>
       </c>
       <c r="W1" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="X1" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="Y1" t="s">
         <v>51</v>
       </c>
       <c r="Z1" s="52" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="AA1" t="s">
         <v>11</v>
@@ -3255,7 +3209,7 @@
         <v>45</v>
       </c>
       <c r="AQ1" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="AR1" s="52" t="s">
         <v>57</v>
@@ -3291,24 +3245,24 @@
         <v>60</v>
       </c>
       <c r="BC1" s="53" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="BD1" s="53" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="BE1" s="53" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="BF1" s="53" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="BG1" s="52" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:AQ2" si="0">+COUNTA(B3:B1048576)</f>
@@ -3545,178 +3499,178 @@
     </row>
     <row r="3" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C3" s="52" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D3" s="52" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="E3" s="52" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="F3" s="52" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="G3" s="52" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="H3" s="52" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="I3" s="52" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="J3" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="K3" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="L3" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="M3" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="N3" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="O3" s="52" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="P3" s="52" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="Q3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="R3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="S3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="T3" s="52" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="U3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="V3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="W3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="X3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="Y3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="Z3" s="52" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="AA3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="AB3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="AC3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="AD3" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="AE3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="AF3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="AG3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="AH3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="AI3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="AJ3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="AK3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="AL3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="AM3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="AN3" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="AO3" s="52" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="AP3" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="AQ3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="AR3" s="52" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="AS3" s="52" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="AT3" s="52" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="AU3" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="AV3" s="52" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="AW3" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="AX3" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="AY3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="AZ3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="BA3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="BB3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="BC3" s="53" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="BD3" s="53" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="BE3" s="53" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="BF3" s="53" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="BG3" s="52" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.3">
@@ -3728,71 +3682,71 @@
       <c r="H4" s="52"/>
       <c r="I4" s="52"/>
       <c r="M4" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="O4" s="52"/>
       <c r="P4" s="52"/>
       <c r="R4" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="T4" s="52"/>
       <c r="V4" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="W4" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="X4" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="Y4" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="Z4" s="52"/>
       <c r="AB4" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="AM4" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="AO4" s="52"/>
       <c r="AQ4" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="AR4" s="52" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="AS4" s="52" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="AT4" s="52"/>
       <c r="AV4" s="52" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="AY4" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="AZ4" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="BA4" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="BB4" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="BC4" s="53"/>
       <c r="BD4" s="53" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="BE4" s="53" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="BF4" s="53" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="BG4" s="52" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:59" x14ac:dyDescent="0.3">
@@ -3807,24 +3761,24 @@
       <c r="P5" s="52"/>
       <c r="T5" s="52"/>
       <c r="V5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="Y5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="Z5" s="52"/>
       <c r="AM5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="AO5" s="52"/>
       <c r="AQ5" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="AR5" s="52" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="AS5" s="52" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="AT5" s="52"/>
       <c r="AV5" s="52"/>

</xml_diff>

<commit_message>
Update Uncertainty Table in the Interface_RDM and a few paths in the experiment_manager
</commit_message>
<xml_diff>
--- a/src/Interface_RDM.xlsx
+++ b/src/Interface_RDM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\AFR_RDM\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0EA1DE-0EAF-468A-B784-60013FB78924}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7334C7E-EF27-48C5-AC0D-1306199319D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="727" activeTab="3" xr2:uid="{A38498C0-325E-4D75-9B65-6D8B75ECDFF0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="727" activeTab="1" xr2:uid="{A38498C0-325E-4D75-9B65-6D8B75ECDFF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Uncertainty_Table" sheetId="13" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="To_Print" sheetId="12" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Uncertainty_Table!$A$1:$N$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Uncertainty_Table!$A$1:$N$14</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="180">
   <si>
     <t>X_Num</t>
   </si>
@@ -613,12 +613,6 @@
   </si>
   <si>
     <t>Collection rate</t>
-  </si>
-  <si>
-    <t>WSTEGN</t>
-  </si>
-  <si>
-    <t>LWTEGN</t>
   </si>
   <si>
     <t>Output Activity Ratio</t>
@@ -658,24 +652,9 @@
     <t>Fixed Cost of ICE vehicles technologies</t>
   </si>
   <si>
-    <t>TRAELCCARCUR ; TRAELCCARNEW ; TRAELCMCYCUR ; TRAELCMCYNEW ; TRAELCMNBCUR ; 
-TRAELCMNBNEW ; TRAELCBUSCUR ; TRAELCBUSNEW ; TRAELCLTRCUR ; TRAELCLTRNEW ; 
-TRAELCMTRCUR ; TRAELCMTRNEW ; TRAELCHTRCUR ; TRAELCHTRNEW</t>
-  </si>
-  <si>
-    <t>TRAGASCARCUR ; TRADSLCARCUR ; TRAGSHCARCUR ; TRAGASCARNEW ; TRALPGCARNEW
- ; TRADSLCARNEW ; TRAGSHCARNEW ; TRAGASMCYCUR ; TRAGASMCYNEW ; TRADSLMCYNEW ; TRAGASMNBCUR ; TRADSLMNBCUR ; TRAGASMNBNEW ; TRALPGMNBNEW ; TRADSLMNBNEW ; TRADSHMNBNEW ; TRADSLBUSCUR ;  TRADSLBUSNEW ; TRALPGBUSNEW ; TRADSLBUSNEW ; TRAGASLTRCUR ; TRADSLLTRCUR
-; TRAGASLTRNEW ; TRADSLLTRNEW ; TRADSHLTRNEW ; TRADSLMTRCUR ; 
-TRADSLMTRNEW ; TRADSKHTRCUR ; TRADSLHTRNEW</t>
-  </si>
-  <si>
     <t>Demand Growth</t>
   </si>
   <si>
-    <t>RESLGTR ; RESLGTU ; RESCKNR ; RESCKNU ; RESSPHR ; RESWTHR ; RESWTHU ; RESCOLU ; 
-RESELCOTHR ; RESELCOTHU</t>
-  </si>
-  <si>
     <t>Changes in demand magnitude</t>
   </si>
   <si>
@@ -688,30 +667,18 @@
     <t>Fixed Cost of crops technologies</t>
   </si>
   <si>
-    <t>BAU</t>
-  </si>
-  <si>
     <t>Time_Series</t>
   </si>
   <si>
     <t>Final_Value</t>
   </si>
   <si>
-    <t>Import Cost of biomass</t>
-  </si>
-  <si>
-    <t>IMPBIO</t>
-  </si>
-  <si>
     <t>Input Activity Ratio</t>
   </si>
   <si>
     <t>Activity ratio of inputs</t>
   </si>
   <si>
-    <t>WSTCOL</t>
-  </si>
-  <si>
     <t xml:space="preserve"> INDOTHPLT ; INDMTRPLT ;  INDCHMPLT ; INDFBTPLT</t>
   </si>
   <si>
@@ -737,6 +704,33 @@
   </si>
   <si>
     <t>cbc</t>
+  </si>
+  <si>
+    <t>Scenario1</t>
+  </si>
+  <si>
+    <t>WSTGEN</t>
+  </si>
+  <si>
+    <t>COLWST</t>
+  </si>
+  <si>
+    <t>COLLWT</t>
+  </si>
+  <si>
+    <t>LWTGEN</t>
+  </si>
+  <si>
+    <t>LNDPLAHR ; LNDPLALR ; LNDMAIHR ; LNDMAILR ; LNDCASHR ; LNDCASLR ; LNDBEAHR ; LNDBEALR ; LNDCOFHR ; LNDCOFLR ; LNDGROHR ; LNDGROLR ; LNDPTSHR ; LNDPTSLR ; LNDSUNHR ; LNDSUNLR ; LNDOTCHR ; LNDOTCLR ; LNDSORHR ; LNDSORLR ; LNDSESHR ; LNDSESLR ; LNDRICHR ; LNDRICHI ; LNDRICLR; LNDSOYHR ; LNDSOYLR ; LNDVEGHR ; LNDVEGLR</t>
+  </si>
+  <si>
+    <t>TRAELCCARCUR ; TRAELCCARNEW ; TRAELCMCYCUR ; TRAELCMCYNEW ; TRAELCMNBCUR ; TRAELCMNBNEW ; TRAELCBUSCUR ; TRAELCBUSNEW ; TRAELCLTRCUR ; TRAELCLTRNEW ; TRAELCMTRCUR ; TRAELCMTRNEW ; TRAELCHTRCUR ; TRAELCHTRNEW</t>
+  </si>
+  <si>
+    <t>RESLGTR ; RESLGTU ; RESCKNR ; RESCKNU ; RESSPHR ; RESWTHR ; RESWTHU ; RESCOLU ; RESELCOTHR ; RESELCOTHU</t>
+  </si>
+  <si>
+    <t>TRADSLCARCUR ; TRALPGCARNEW ; TRADSLCARNEW ; TRADSLMCYNEW ; TRADSLMNBCUR ; TRALPGMNBNEW ; TRADSLMNBNEW ; TRADSHMNBNEW ; TRADSLBUSCUR ; TRADSLBUSNEW ; TRALPGBUSNEW ; TRADSLBUSNEW ; TRADSLLTRCUR ; TRADSLLTRNEW ; TRADSHLTRNEW ; TRADSLMTRCUR ; TRADSLMTRNEW ; TRADSLHTRCUR ; TRADSLHTRNEW</t>
   </si>
 </sst>
 </file>
@@ -1314,31 +1308,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B5B787-8749-47D9-9D7A-FB53FE5A30D3}">
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView topLeftCell="B8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" style="16" customWidth="1"/>
+    <col min="2" max="2" width="28.33203125" style="16" customWidth="1"/>
     <col min="3" max="3" width="44" style="17" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" style="22" customWidth="1"/>
-    <col min="6" max="7" width="32.140625" style="22" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" style="22" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" style="22" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" style="22" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" style="22" customWidth="1"/>
+    <col min="6" max="7" width="32.109375" style="22" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" style="22" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" style="22" customWidth="1"/>
     <col min="10" max="10" width="54" style="22" customWidth="1"/>
-    <col min="11" max="11" width="79.7109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="79.6640625" style="23" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="49" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="45.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45.88671875" style="22" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="44" style="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.85546875" style="21"/>
+    <col min="15" max="16384" width="8.88671875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1382,7 +1376,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="16">
         <v>1</v>
       </c>
@@ -1390,16 +1384,16 @@
         <v>140</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D2" s="16" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E2" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F2" s="16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G2" s="16">
         <v>2026</v>
@@ -1414,10 +1408,10 @@
         <v>119</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>141</v>
+        <v>172</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="M2" s="16" t="s">
         <v>11</v>
@@ -1426,24 +1420,25 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="16">
+        <f>1+A2</f>
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>140</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D3" s="16" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G3" s="16">
         <v>2026</v>
@@ -1458,10 +1453,10 @@
         <v>119</v>
       </c>
       <c r="K3" s="17" t="s">
-        <v>142</v>
+        <v>175</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="M3" s="16" t="s">
         <v>11</v>
@@ -1470,165 +1465,169 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="16" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
+        <f t="shared" ref="A4:A15" si="0">1+A3</f>
         <v>3</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G4" s="16">
         <v>2026</v>
       </c>
       <c r="H4" s="16">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="I4" s="16">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="K4" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="L4" s="17" t="s">
-        <v>147</v>
-      </c>
-      <c r="M4" s="16">
+        <v>144</v>
+      </c>
+      <c r="L4" s="17">
         <v>1</v>
       </c>
       <c r="N4" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="16" customFormat="1" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G5" s="16">
         <v>2026</v>
       </c>
       <c r="H5" s="16">
-        <v>0.9</v>
+        <v>0.8</v>
       </c>
       <c r="I5" s="16">
-        <v>1.3</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>14</v>
+        <v>1.4</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="K5" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="L5" s="17">
-        <v>1</v>
+        <v>176</v>
+      </c>
+      <c r="L5" s="17" t="s">
+        <v>11</v>
       </c>
       <c r="N5" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="16" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="16">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F6" s="16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G6" s="16">
         <v>2026</v>
       </c>
       <c r="H6" s="16">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="I6" s="16">
         <v>1.4</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="24" t="s">
-        <v>146</v>
-      </c>
-      <c r="L6" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="16" t="s">
         <v>11</v>
       </c>
       <c r="N6" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="16">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G7" s="16">
         <v>2026</v>
       </c>
       <c r="H7" s="16">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="I7" s="16">
-        <v>1.4</v>
+        <v>1.2</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="K7" s="25" t="s">
-        <v>155</v>
+        <v>177</v>
       </c>
       <c r="L7" s="16" t="s">
         <v>11</v>
@@ -1640,24 +1639,25 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" s="16" customFormat="1" ht="112.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G8" s="16">
         <v>2026</v>
@@ -1669,10 +1669,10 @@
         <v>1.2</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K8" s="25" t="s">
-        <v>155</v>
+        <v>10</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>179</v>
       </c>
       <c r="L8" s="16" t="s">
         <v>11</v>
@@ -1684,24 +1684,25 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="16" customFormat="1" ht="112.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G9" s="16">
         <v>2026</v>
@@ -1710,13 +1711,13 @@
         <v>0.9</v>
       </c>
       <c r="I9" s="16">
-        <v>1.2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="K9" s="17" t="s">
-        <v>156</v>
+        <v>179</v>
       </c>
       <c r="L9" s="16" t="s">
         <v>11</v>
@@ -1728,24 +1729,25 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="16" customFormat="1" ht="120" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" s="16" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>154</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G10" s="16">
         <v>2026</v>
@@ -1754,13 +1756,13 @@
         <v>0.9</v>
       </c>
       <c r="I10" s="16">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="J10" s="16" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="K10" s="17" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="L10" s="16" t="s">
         <v>11</v>
@@ -1772,42 +1774,43 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="16" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="20" customFormat="1" ht="73.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C11" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="F11" s="16" t="s">
         <v>159</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>165</v>
       </c>
       <c r="G11" s="16">
         <v>2026</v>
       </c>
       <c r="H11" s="16">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="I11" s="16">
-        <v>1.2</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>27</v>
+        <v>1.5</v>
+      </c>
+      <c r="J11" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="L11" s="16" t="s">
-        <v>11</v>
+        <v>164</v>
+      </c>
+      <c r="L11" s="17">
+        <v>1</v>
       </c>
       <c r="M11" s="16" t="s">
         <v>11</v>
@@ -1816,68 +1819,70 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="20" customFormat="1" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" s="20" customFormat="1" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>160</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>174</v>
+        <v>161</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G12" s="16">
         <v>2026</v>
       </c>
       <c r="H12" s="16">
-        <v>0.7</v>
+        <v>0.9</v>
       </c>
       <c r="I12" s="16">
-        <v>1.5</v>
+        <v>1.2</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="L12" s="17">
-        <v>1</v>
-      </c>
-      <c r="M12" s="16" t="s">
-        <v>11</v>
+        <v>43</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="M12" s="16">
+        <v>1</v>
       </c>
       <c r="N12" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="20" customFormat="1" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="20" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="16">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D13" s="16" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G13" s="16">
         <v>2026</v>
@@ -1886,42 +1891,43 @@
         <v>0.8</v>
       </c>
       <c r="I13" s="16">
-        <v>1.4</v>
-      </c>
-      <c r="J13" s="17" t="s">
-        <v>14</v>
+        <v>1.5</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="K13" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="L13" s="17">
-        <v>1</v>
-      </c>
-      <c r="M13" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="L13" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="M13" s="17" t="s">
         <v>11</v>
       </c>
       <c r="N13" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="20" customFormat="1" ht="61.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="20" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="16">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>169</v>
       </c>
       <c r="D14" s="16" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G14" s="16">
         <v>2026</v>
@@ -1930,42 +1936,43 @@
         <v>0.9</v>
       </c>
       <c r="I14" s="16">
-        <v>1.2</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="K14" s="16" t="s">
-        <v>171</v>
+        <v>1.3</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="17" t="s">
+        <v>167</v>
       </c>
       <c r="L14" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="M14" s="16">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="M14" s="17" t="s">
+        <v>11</v>
       </c>
       <c r="N14" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A15" s="16">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G15" s="16">
         <v>2026</v>
@@ -1974,73 +1981,29 @@
         <v>0.8</v>
       </c>
       <c r="I15" s="16">
-        <v>1.5</v>
-      </c>
-      <c r="J15" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="K15" s="17" t="s">
-        <v>175</v>
+        <v>1.2</v>
+      </c>
+      <c r="J15" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" s="24" t="s">
+        <v>144</v>
       </c>
       <c r="L15" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="M15" s="17" t="s">
-        <v>11</v>
+        <v>145</v>
+      </c>
+      <c r="M15" s="16">
+        <v>1</v>
       </c>
       <c r="N15" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="20" customFormat="1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="16">
-        <v>15</v>
-      </c>
-      <c r="B16" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="G16" s="16">
-        <v>2026</v>
-      </c>
-      <c r="H16" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="I16" s="16">
-        <v>1.3</v>
-      </c>
-      <c r="J16" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="K16" s="17" t="s">
-        <v>176</v>
-      </c>
-      <c r="L16" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="M16" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="N16" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F50" s="26"/>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F48" s="26"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N16" xr:uid="{95B5B787-8749-47D9-9D7A-FB53FE5A30D3}"/>
+  <autoFilter ref="A1:N14" xr:uid="{95B5B787-8749-47D9-9D7A-FB53FE5A30D3}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -2051,21 +2014,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8EBD12E-40AD-42BC-9E38-C5D5CF6C4FA5}">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="15.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2094,9 +2057,9 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>20</v>
@@ -2105,17 +2068,19 @@
         <v>1</v>
       </c>
       <c r="D2" s="8">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E2" s="9">
         <v>8</v>
       </c>
-      <c r="F2" s="12"/>
+      <c r="F2" s="12" t="s">
+        <v>24</v>
+      </c>
       <c r="G2" s="2" t="s">
         <v>24</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>139</v>
@@ -2134,66 +2099,66 @@
       <selection activeCell="Y3" sqref="Y3:Y5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="18" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="23" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.5546875" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="22" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="18" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="23.109375" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="38" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="35.88671875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="26" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="7.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>124</v>
       </c>
@@ -2372,7 +2337,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -2609,7 +2574,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>126</v>
       </c>
@@ -2785,7 +2750,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
       <c r="C4" s="14"/>
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
@@ -2861,7 +2826,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
       <c r="C5" s="14"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
@@ -2910,17 +2875,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C82A0652-0771-4DB6-84D0-EEBD0FFCEFAB}">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -2928,12 +2893,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -2941,7 +2906,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -2949,12 +2914,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -2962,7 +2927,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -2970,7 +2935,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -2978,22 +2943,22 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -3001,37 +2966,37 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -3039,7 +3004,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>89</v>
       </c>
@@ -3047,92 +3012,92 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>107</v>
       </c>
@@ -3140,17 +3105,17 @@
         <v>112</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>110</v>
       </c>
@@ -3161,6 +3126,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BAD73B84EC2FBA4AB6031CFB79C3D0E0" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1d8e6320e34b5f71545ca20c1fb39b21">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c4f98862-adfd-4d9c-a945-852f80f0eb51" xmlns:ns3="b9355cc9-2d41-4aa9-bfbc-bd016a1e1a01" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f42cd320e09c56919cd7e955403e252" ns2:_="" ns3:_="">
     <xsd:import namespace="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
@@ -3377,15 +3351,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -3397,6 +3362,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAAAB53-0ECA-470A-A9D1-4E2A413E8F82}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED653E30-6791-4489-AE1B-B6DFD5392ED4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3415,14 +3388,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAAAB53-0ECA-470A-A9D1-4E2A413E8F82}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6E40288-91D1-4CD6-86D1-178CC2AEE7EC}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Make changes to copy results into the 1_Experiment folder
</commit_message>
<xml_diff>
--- a/src/Interface_RDM.xlsx
+++ b/src/Interface_RDM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\AFR_RDM\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7334C7E-EF27-48C5-AC0D-1306199319D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93E7BCD-7145-4ED9-A779-96037E178CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="727" activeTab="1" xr2:uid="{A38498C0-325E-4D75-9B65-6D8B75ECDFF0}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="727" xr2:uid="{A38498C0-325E-4D75-9B65-6D8B75ECDFF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Uncertainty_Table" sheetId="13" r:id="rId1"/>
@@ -55,7 +55,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Climate Lead Group:</t>
         </r>
@@ -64,7 +64,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Options:
@@ -84,7 +84,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Climate Lead Group:</t>
         </r>
@@ -93,7 +93,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Check "Params_Sets_Vari" for each parameter involved. You need put sets related with the parameter in the same order as you see in the sheet.
@@ -109,7 +109,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Climate Lead Group:</t>
         </r>
@@ -118,7 +118,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Check "Params_Sets_Vari" for each parameter involved. You need put sets related with the parameter in the same order as you see in the sheet.
@@ -134,7 +134,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Climate Lead Group:</t>
         </r>
@@ -143,7 +143,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Check "Params_Sets_Vari" for each parameter involved. You need put sets related with the parameter in the same order as you see in the sheet.
@@ -169,7 +169,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Climate Lead Group:</t>
         </r>
@@ -178,7 +178,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Parameters paint in brown can not do a variation in RDM experiment.</t>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="182">
   <si>
     <t>X_Num</t>
   </si>
@@ -706,9 +706,6 @@
     <t>cbc</t>
   </si>
   <si>
-    <t>Scenario1</t>
-  </si>
-  <si>
     <t>WSTGEN</t>
   </si>
   <si>
@@ -731,6 +728,15 @@
   </si>
   <si>
     <t>TRADSLCARCUR ; TRALPGCARNEW ; TRADSLCARNEW ; TRADSLMCYNEW ; TRADSLMNBCUR ; TRALPGMNBNEW ; TRADSLMNBNEW ; TRADSHMNBNEW ; TRADSLBUSCUR ; TRADSLBUSNEW ; TRALPGBUSNEW ; TRADSLBUSNEW ; TRADSLLTRCUR ; TRADSLLTRNEW ; TRADSHLTRNEW ; TRADSLMTRCUR ; TRADSLMTRNEW ; TRADSLHTRCUR ; TRADSLHTRNEW</t>
+  </si>
+  <si>
+    <t>Region</t>
+  </si>
+  <si>
+    <t>UGA</t>
+  </si>
+  <si>
+    <t>BAU ; Scenario1</t>
   </si>
 </sst>
 </file>
@@ -758,13 +764,13 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -811,7 +817,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -920,11 +926,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -952,7 +982,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -985,6 +1014,12 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1310,697 +1345,697 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B5B787-8749-47D9-9D7A-FB53FE5A30D3}">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView topLeftCell="B8" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="16" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" style="16" customWidth="1"/>
-    <col min="3" max="3" width="44" style="17" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" style="22" customWidth="1"/>
-    <col min="5" max="5" width="27.44140625" style="22" customWidth="1"/>
-    <col min="6" max="7" width="32.109375" style="22" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" style="22" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" style="22" customWidth="1"/>
-    <col min="10" max="10" width="54" style="22" customWidth="1"/>
-    <col min="11" max="11" width="79.6640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="49" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="45.88671875" style="22" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="44" style="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="21"/>
+    <col min="1" max="1" width="9.5703125" style="15" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" style="15" customWidth="1"/>
+    <col min="3" max="3" width="44" style="16" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="21" customWidth="1"/>
+    <col min="6" max="7" width="32.140625" style="21" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="21" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" style="21" customWidth="1"/>
+    <col min="10" max="10" width="54" style="21" customWidth="1"/>
+    <col min="11" max="11" width="79.7109375" style="22" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="49" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="45.85546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="44" style="22" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:14" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="19" t="s">
+      <c r="B1" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="18" t="s">
         <v>136</v>
       </c>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="N1" s="18" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="16">
-        <v>1</v>
-      </c>
-      <c r="B2" s="16" t="s">
+    <row r="2" spans="1:14" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <v>1</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G2" s="15">
+        <v>2026</v>
+      </c>
+      <c r="H2" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="I2" s="15">
+        <v>1</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="K2" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="G2" s="16">
-        <v>2026</v>
-      </c>
-      <c r="H2" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="I2" s="16">
-        <v>1</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="K2" s="17" t="s">
+      <c r="L2" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="L2" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="16">
+    <row r="3" spans="1:14" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
         <f>1+A2</f>
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>140</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="E3" s="16" t="s">
+      <c r="D3" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E3" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="G3" s="16">
+      <c r="G3" s="15">
         <v>2026</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="15">
         <v>0.6</v>
       </c>
-      <c r="I3" s="16">
-        <v>1</v>
-      </c>
-      <c r="J3" s="16" t="s">
+      <c r="I3" s="15">
+        <v>1</v>
+      </c>
+      <c r="J3" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="K3" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="L3" s="17" t="s">
+      <c r="K3" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="M3" s="16" t="s">
+      <c r="L3" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="M3" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="16" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16">
+    <row r="4" spans="1:14" s="15" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
         <f t="shared" ref="A4:A15" si="0">1+A3</f>
         <v>3</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="E4" s="16" t="s">
+      <c r="D4" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="15">
         <v>2026</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="15">
         <v>0.9</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="15">
         <v>1.3</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="L4" s="17">
-        <v>1</v>
-      </c>
-      <c r="N4" s="17" t="s">
+      <c r="L4" s="16">
+        <v>1</v>
+      </c>
+      <c r="N4" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="16" customFormat="1" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16">
+    <row r="5" spans="1:14" s="15" customFormat="1" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>148</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="D5" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="E5" s="16" t="s">
+      <c r="D5" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E5" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="15">
         <v>2026</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="15">
         <v>0.8</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="15">
         <v>1.4</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="J5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="K5" s="24" t="s">
+      <c r="K5" s="23" t="s">
+        <v>175</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G6" s="15">
+        <v>2026</v>
+      </c>
+      <c r="H6" s="15">
+        <v>0.7</v>
+      </c>
+      <c r="I6" s="15">
+        <v>1.4</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K6" s="24" t="s">
         <v>176</v>
       </c>
-      <c r="L5" s="17" t="s">
+      <c r="L6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="17" t="s">
+      <c r="M6" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6" s="16">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" s="16" t="s">
+    <row r="7" spans="1:14" s="15" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G7" s="15">
+        <v>2026</v>
+      </c>
+      <c r="H7" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="I7" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="J7" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>176</v>
+      </c>
+      <c r="L7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="15" customFormat="1" ht="112.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="E6" s="16" t="s">
+      <c r="C8" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F8" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G8" s="15">
         <v>2026</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H8" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="I8" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="15" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F9" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G9" s="15">
+        <v>2026</v>
+      </c>
+      <c r="H9" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="I9" s="15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="15" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F10" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G10" s="15">
+        <v>2026</v>
+      </c>
+      <c r="H10" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="I10" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="J10" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="L10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="M10" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="19" customFormat="1" ht="73.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G11" s="15">
+        <v>2026</v>
+      </c>
+      <c r="H11" s="15">
         <v>0.7</v>
       </c>
-      <c r="I6" s="16">
-        <v>1.4</v>
-      </c>
-      <c r="J6" s="16" t="s">
+      <c r="I11" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="L11" s="16">
+        <v>1</v>
+      </c>
+      <c r="M11" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="19" customFormat="1" ht="61.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F12" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G12" s="15">
+        <v>2026</v>
+      </c>
+      <c r="H12" s="15">
+        <v>0.9</v>
+      </c>
+      <c r="I12" s="15">
+        <v>1.2</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="M12" s="15">
+        <v>1</v>
+      </c>
+      <c r="N12" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G13" s="15">
+        <v>2026</v>
+      </c>
+      <c r="H13" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="I13" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="J13" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="K6" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="L6" s="16" t="s">
+      <c r="K13" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="L13" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="16" t="s">
+      <c r="M13" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="N6" s="17" t="s">
+      <c r="N13" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>150</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="E7" s="16" t="s">
+    <row r="14" spans="1:14" s="19" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F14" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G14" s="15">
         <v>2026</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H14" s="15">
         <v>0.9</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I14" s="15">
+        <v>1.3</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="M14" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="N14" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="G15" s="15">
+        <v>2026</v>
+      </c>
+      <c r="H15" s="15">
+        <v>0.8</v>
+      </c>
+      <c r="I15" s="15">
         <v>1.2</v>
       </c>
-      <c r="J7" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="25" t="s">
-        <v>177</v>
-      </c>
-      <c r="L7" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="M7" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="N7" s="17" t="s">
+      <c r="J15" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" s="23" t="s">
+        <v>144</v>
+      </c>
+      <c r="L15" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="M15" s="15">
+        <v>1</v>
+      </c>
+      <c r="N15" s="16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="16" customFormat="1" ht="112.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="16">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="E8" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="G8" s="16">
-        <v>2026</v>
-      </c>
-      <c r="H8" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="I8" s="16">
-        <v>1.2</v>
-      </c>
-      <c r="J8" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="N8" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" s="16" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="16">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>148</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="G9" s="16">
-        <v>2026</v>
-      </c>
-      <c r="H9" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="I9" s="16">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="K9" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="L9" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="M9" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="N9" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" s="16" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="G10" s="16">
-        <v>2026</v>
-      </c>
-      <c r="H10" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="I10" s="16">
-        <v>1.2</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="K10" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="L10" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="M10" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="N10" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" s="20" customFormat="1" ht="73.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>165</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="G11" s="16">
-        <v>2026</v>
-      </c>
-      <c r="H11" s="16">
-        <v>0.7</v>
-      </c>
-      <c r="I11" s="16">
-        <v>1.5</v>
-      </c>
-      <c r="J11" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="K11" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="L11" s="17">
-        <v>1</v>
-      </c>
-      <c r="M11" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="N11" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" s="20" customFormat="1" ht="61.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="C12" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="D12" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="G12" s="16">
-        <v>2026</v>
-      </c>
-      <c r="H12" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="I12" s="16">
-        <v>1.2</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="K12" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="L12" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="M12" s="16">
-        <v>1</v>
-      </c>
-      <c r="N12" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" s="20" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A13" s="16">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="G13" s="16">
-        <v>2026</v>
-      </c>
-      <c r="H13" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="I13" s="16">
-        <v>1.5</v>
-      </c>
-      <c r="J13" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="L13" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="M13" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="N13" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="20" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="16">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="D14" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="G14" s="16">
-        <v>2026</v>
-      </c>
-      <c r="H14" s="16">
-        <v>0.9</v>
-      </c>
-      <c r="I14" s="16">
-        <v>1.3</v>
-      </c>
-      <c r="J14" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="K14" s="17" t="s">
-        <v>167</v>
-      </c>
-      <c r="L14" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="M14" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="N14" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="16">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>146</v>
-      </c>
-      <c r="D15" s="16" t="s">
-        <v>171</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="G15" s="16">
-        <v>2026</v>
-      </c>
-      <c r="H15" s="16">
-        <v>0.8</v>
-      </c>
-      <c r="I15" s="16">
-        <v>1.2</v>
-      </c>
-      <c r="J15" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="K15" s="24" t="s">
-        <v>144</v>
-      </c>
-      <c r="L15" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="M15" s="16">
-        <v>1</v>
-      </c>
-      <c r="N15" s="17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="48" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F48" s="26"/>
+    <row r="48" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F48" s="25"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:N14" xr:uid="{95B5B787-8749-47D9-9D7A-FB53FE5A30D3}"/>
@@ -2012,23 +2047,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8EBD12E-40AD-42BC-9E38-C5D5CF6C4FA5}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -2053,11 +2088,14 @@
       <c r="H1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="10" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J1" s="27" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>20</v>
       </c>
@@ -2068,7 +2106,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="8">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E2" s="9">
         <v>8</v>
@@ -2084,6 +2122,9 @@
       </c>
       <c r="I2" s="2" t="s">
         <v>139</v>
+      </c>
+      <c r="J2" s="26" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2099,91 +2140,91 @@
       <selection activeCell="Y3" sqref="Y3:Y5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="11" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="18" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="23" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="38" width="44.88671875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="25.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="22.88671875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="22" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="18" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="51" max="51" width="38" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="53" max="54" width="35.88671875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="53" max="54" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="58" max="58" width="26" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="7.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>124</v>
       </c>
       <c r="B1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>35</v>
       </c>
       <c r="J1" t="s">
@@ -2201,10 +2242,10 @@
       <c r="N1" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="13" t="s">
         <v>123</v>
       </c>
       <c r="Q1" t="s">
@@ -2216,7 +2257,7 @@
       <c r="S1" t="s">
         <v>29</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="T1" s="13" t="s">
         <v>46</v>
       </c>
       <c r="U1" t="s">
@@ -2234,7 +2275,7 @@
       <c r="Y1" t="s">
         <v>48</v>
       </c>
-      <c r="Z1" s="14" t="s">
+      <c r="Z1" s="13" t="s">
         <v>117</v>
       </c>
       <c r="AA1" t="s">
@@ -2279,7 +2320,7 @@
       <c r="AN1" t="s">
         <v>28</v>
       </c>
-      <c r="AO1" s="14" t="s">
+      <c r="AO1" s="13" t="s">
         <v>45</v>
       </c>
       <c r="AP1" t="s">
@@ -2288,19 +2329,19 @@
       <c r="AQ1" t="s">
         <v>114</v>
       </c>
-      <c r="AR1" s="14" t="s">
+      <c r="AR1" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="AS1" s="14" t="s">
+      <c r="AS1" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="AT1" s="14" t="s">
+      <c r="AT1" s="13" t="s">
         <v>53</v>
       </c>
       <c r="AU1" t="s">
         <v>44</v>
       </c>
-      <c r="AV1" s="14" t="s">
+      <c r="AV1" s="13" t="s">
         <v>47</v>
       </c>
       <c r="AW1" t="s">
@@ -2321,23 +2362,23 @@
       <c r="BB1" t="s">
         <v>57</v>
       </c>
-      <c r="BC1" s="15" t="s">
+      <c r="BC1" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="BD1" s="15" t="s">
+      <c r="BD1" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="BE1" s="15" t="s">
+      <c r="BE1" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="BF1" s="15" t="s">
+      <c r="BF1" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="BG1" s="14" t="s">
+      <c r="BG1" s="13" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>125</v>
       </c>
@@ -2345,31 +2386,31 @@
         <f t="shared" ref="B2:AQ2" si="0">+COUNTA(B3:B1048576)</f>
         <v>1</v>
       </c>
-      <c r="C2" s="14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="D2" s="14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E2" s="14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F2" s="14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G2" s="14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H2" s="14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I2" s="14">
+      <c r="C2" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="D2" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E2" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F2" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G2" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="H2" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I2" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2393,11 +2434,11 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="O2" s="14">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="P2" s="14">
+      <c r="O2" s="13">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="P2" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2413,7 +2454,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="T2" s="14">
+      <c r="T2" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2437,7 +2478,7 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="Z2" s="14">
+      <c r="Z2" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2497,7 +2538,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="AO2" s="14">
+      <c r="AO2" s="13">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2509,15 +2550,15 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="AR2" s="14">
+      <c r="AR2" s="13">
         <f>+COUNTA(AR3:AR5)</f>
         <v>3</v>
       </c>
-      <c r="AS2" s="14">
+      <c r="AS2" s="13">
         <f>+COUNTA(AS3:AS5)</f>
         <v>3</v>
       </c>
-      <c r="AT2" s="14">
+      <c r="AT2" s="13">
         <f t="shared" ref="AT2:BG2" si="1">+COUNTA(AT3:AT6)</f>
         <v>1</v>
       </c>
@@ -2525,7 +2566,7 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AV2" s="14">
+      <c r="AV2" s="13">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
@@ -2553,50 +2594,50 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="BC2" s="15">
+      <c r="BC2" s="14">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="BD2" s="15">
+      <c r="BD2" s="14">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="BE2" s="15">
+      <c r="BE2" s="14">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="BF2" s="15">
+      <c r="BF2" s="14">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="BG2" s="14">
+      <c r="BG2" s="13">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:59" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:59" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>126</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="13" t="s">
         <v>126</v>
       </c>
       <c r="J3" t="s">
@@ -2614,10 +2655,10 @@
       <c r="N3" t="s">
         <v>130</v>
       </c>
-      <c r="O3" s="14" t="s">
+      <c r="O3" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="P3" s="14" t="s">
+      <c r="P3" s="13" t="s">
         <v>127</v>
       </c>
       <c r="Q3" t="s">
@@ -2629,7 +2670,7 @@
       <c r="S3" t="s">
         <v>131</v>
       </c>
-      <c r="T3" s="14" t="s">
+      <c r="T3" s="13" t="s">
         <v>127</v>
       </c>
       <c r="U3" t="s">
@@ -2647,7 +2688,7 @@
       <c r="Y3" t="s">
         <v>131</v>
       </c>
-      <c r="Z3" s="14" t="s">
+      <c r="Z3" s="13" t="s">
         <v>127</v>
       </c>
       <c r="AA3" t="s">
@@ -2692,7 +2733,7 @@
       <c r="AN3" t="s">
         <v>133</v>
       </c>
-      <c r="AO3" s="14" t="s">
+      <c r="AO3" s="13" t="s">
         <v>133</v>
       </c>
       <c r="AP3" t="s">
@@ -2701,19 +2742,19 @@
       <c r="AQ3" t="s">
         <v>131</v>
       </c>
-      <c r="AR3" s="14" t="s">
+      <c r="AR3" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="AS3" s="14" t="s">
+      <c r="AS3" s="13" t="s">
         <v>131</v>
       </c>
-      <c r="AT3" s="14" t="s">
+      <c r="AT3" s="13" t="s">
         <v>132</v>
       </c>
       <c r="AU3" t="s">
         <v>132</v>
       </c>
-      <c r="AV3" s="14" t="s">
+      <c r="AV3" s="13" t="s">
         <v>127</v>
       </c>
       <c r="AW3" t="s">
@@ -2734,39 +2775,39 @@
       <c r="BB3" t="s">
         <v>131</v>
       </c>
-      <c r="BC3" s="15" t="s">
+      <c r="BC3" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="BD3" s="15" t="s">
+      <c r="BD3" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="BE3" s="15" t="s">
+      <c r="BE3" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="BF3" s="15" t="s">
+      <c r="BF3" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="BG3" s="14" t="s">
+      <c r="BG3" s="13" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="4" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
+    <row r="4" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
       <c r="M4" t="s">
         <v>126</v>
       </c>
-      <c r="O4" s="14"/>
-      <c r="P4" s="14"/>
+      <c r="O4" s="13"/>
+      <c r="P4" s="13"/>
       <c r="R4" t="s">
         <v>126</v>
       </c>
-      <c r="T4" s="14"/>
+      <c r="T4" s="13"/>
       <c r="V4" t="s">
         <v>130</v>
       </c>
@@ -2779,25 +2820,25 @@
       <c r="Y4" t="s">
         <v>130</v>
       </c>
-      <c r="Z4" s="14"/>
+      <c r="Z4" s="13"/>
       <c r="AB4" t="s">
         <v>135</v>
       </c>
       <c r="AM4" t="s">
         <v>133</v>
       </c>
-      <c r="AO4" s="14"/>
+      <c r="AO4" s="13"/>
       <c r="AQ4" t="s">
         <v>133</v>
       </c>
-      <c r="AR4" s="14" t="s">
+      <c r="AR4" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="AS4" s="14" t="s">
+      <c r="AS4" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="AT4" s="14"/>
-      <c r="AV4" s="14" t="s">
+      <c r="AT4" s="13"/>
+      <c r="AV4" s="13" t="s">
         <v>132</v>
       </c>
       <c r="AY4" t="s">
@@ -2812,58 +2853,58 @@
       <c r="BB4" t="s">
         <v>135</v>
       </c>
-      <c r="BC4" s="15"/>
-      <c r="BD4" s="15" t="s">
+      <c r="BC4" s="14"/>
+      <c r="BD4" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="BE4" s="15" t="s">
+      <c r="BE4" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="BF4" s="15" t="s">
+      <c r="BF4" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="BG4" s="14" t="s">
+      <c r="BG4" s="13" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="5" spans="1:59" x14ac:dyDescent="0.3">
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="T5" s="14"/>
+    <row r="5" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="O5" s="13"/>
+      <c r="P5" s="13"/>
+      <c r="T5" s="13"/>
       <c r="V5" t="s">
         <v>135</v>
       </c>
       <c r="Y5" t="s">
         <v>135</v>
       </c>
-      <c r="Z5" s="14"/>
+      <c r="Z5" s="13"/>
       <c r="AM5" t="s">
         <v>135</v>
       </c>
-      <c r="AO5" s="14"/>
+      <c r="AO5" s="13"/>
       <c r="AQ5" t="s">
         <v>135</v>
       </c>
-      <c r="AR5" s="14" t="s">
+      <c r="AR5" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="AS5" s="14" t="s">
+      <c r="AS5" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="AT5" s="14"/>
-      <c r="AV5" s="14"/>
-      <c r="BC5" s="15"/>
-      <c r="BD5" s="15"/>
-      <c r="BE5" s="15"/>
-      <c r="BF5" s="15"/>
-      <c r="BG5" s="14"/>
+      <c r="AT5" s="13"/>
+      <c r="AV5" s="13"/>
+      <c r="BC5" s="14"/>
+      <c r="BD5" s="14"/>
+      <c r="BE5" s="14"/>
+      <c r="BF5" s="14"/>
+      <c r="BG5" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2879,13 +2920,13 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -2893,12 +2934,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>72</v>
       </c>
@@ -2906,7 +2947,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -2914,12 +2955,12 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>75</v>
       </c>
@@ -2927,7 +2968,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>76</v>
       </c>
@@ -2935,7 +2976,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>77</v>
       </c>
@@ -2943,22 +2984,22 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>81</v>
       </c>
@@ -2966,37 +3007,37 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>88</v>
       </c>
@@ -3004,7 +3045,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>89</v>
       </c>
@@ -3012,92 +3053,92 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>107</v>
       </c>
@@ -3105,17 +3146,17 @@
         <v>112</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>110</v>
       </c>
@@ -3126,6 +3167,16 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c4f98862-adfd-4d9c-a945-852f80f0eb51">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3134,7 +3185,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BAD73B84EC2FBA4AB6031CFB79C3D0E0" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1d8e6320e34b5f71545ca20c1fb39b21">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c4f98862-adfd-4d9c-a945-852f80f0eb51" xmlns:ns3="b9355cc9-2d41-4aa9-bfbc-bd016a1e1a01" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f42cd320e09c56919cd7e955403e252" ns2:_="" ns3:_="">
     <xsd:import namespace="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
@@ -3351,17 +3402,17 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c4f98862-adfd-4d9c-a945-852f80f0eb51">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6E40288-91D1-4CD6-86D1-178CC2AEE7EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAAAB53-0ECA-470A-A9D1-4E2A413E8F82}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -3369,7 +3420,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED653E30-6791-4489-AE1B-B6DFD5392ED4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3386,14 +3437,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6E40288-91D1-4CD6-86D1-178CC2AEE7EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Enhance DVC pipeline and fix Windows pip install bug
- Fix shell redirection bug: Quote pip package specs to prevent >=
  being interpreted as file redirect on Windows (was creating 0.3.8
  and 3.0.0 files with pip output)
- Split PRIM execution into two stages: prim_files_creator and prim_analysis
- Correct PRIM script execution order: t3f1 → t3f2 → t3f3 → t3f4
- Add unbuffered output (-u flag) to subprocess calls for real-time logs
- Update README with complete DVC automation documentation
- Add .gitignore files for experiment outputs and PRIM results
- Remove deprecated run_prim.py in favor of separate wrapper scripts
</commit_message>
<xml_diff>
--- a/src/Interface_RDM.xlsx
+++ b/src/Interface_RDM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\AFR_RDM\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93E7BCD-7145-4ED9-A779-96037E178CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18ECDC62-1520-4DC9-B4F8-369EBD1541B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="727" xr2:uid="{A38498C0-325E-4D75-9B65-6D8B75ECDFF0}"/>
+    <workbookView xWindow="-20772" yWindow="2268" windowWidth="17280" windowHeight="8880" tabRatio="727" activeTab="1" xr2:uid="{A38498C0-325E-4D75-9B65-6D8B75ECDFF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Uncertainty_Table" sheetId="13" r:id="rId1"/>
@@ -703,9 +703,6 @@
     <t>Capital Cost of Steel direct electric arc furnance with natural gas technologies , Capital Cost of cement industry kilns without CCS</t>
   </si>
   <si>
-    <t>cbc</t>
-  </si>
-  <si>
     <t>WSTGEN</t>
   </si>
   <si>
@@ -736,7 +733,10 @@
     <t>UGA</t>
   </si>
   <si>
-    <t>BAU ; Scenario1</t>
+    <t>cplex</t>
+  </si>
+  <si>
+    <t>Scenario1</t>
   </si>
 </sst>
 </file>
@@ -1345,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B5B787-8749-47D9-9D7A-FB53FE5A30D3}">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D15"/>
+    <sheetView topLeftCell="A11" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1443,10 +1443,10 @@
         <v>119</v>
       </c>
       <c r="K2" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="L2" s="16" t="s">
         <v>171</v>
-      </c>
-      <c r="L2" s="16" t="s">
-        <v>172</v>
       </c>
       <c r="M2" s="15" t="s">
         <v>11</v>
@@ -1488,10 +1488,10 @@
         <v>119</v>
       </c>
       <c r="K3" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L3" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M3" s="15" t="s">
         <v>11</v>
@@ -1575,7 +1575,7 @@
         <v>13</v>
       </c>
       <c r="K5" s="23" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L5" s="16" t="s">
         <v>11</v>
@@ -1617,7 +1617,7 @@
         <v>10</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L6" s="15" t="s">
         <v>11</v>
@@ -1662,7 +1662,7 @@
         <v>13</v>
       </c>
       <c r="K7" s="24" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L7" s="15" t="s">
         <v>11</v>
@@ -1707,7 +1707,7 @@
         <v>10</v>
       </c>
       <c r="K8" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L8" s="15" t="s">
         <v>11</v>
@@ -1752,7 +1752,7 @@
         <v>13</v>
       </c>
       <c r="K9" s="16" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="L9" s="15" t="s">
         <v>11</v>
@@ -1797,7 +1797,7 @@
         <v>27</v>
       </c>
       <c r="K10" s="16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="L10" s="15" t="s">
         <v>11</v>
@@ -2049,7 +2049,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8EBD12E-40AD-42BC-9E38-C5D5CF6C4FA5}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -2092,12 +2092,12 @@
         <v>70</v>
       </c>
       <c r="J1" s="27" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>20</v>
@@ -2106,7 +2106,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="8">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E2" s="9">
         <v>8</v>
@@ -2118,13 +2118,13 @@
         <v>24</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>139</v>
       </c>
       <c r="J2" s="26" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -3167,25 +3167,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c4f98862-adfd-4d9c-a945-852f80f0eb51">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BAD73B84EC2FBA4AB6031CFB79C3D0E0" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1d8e6320e34b5f71545ca20c1fb39b21">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c4f98862-adfd-4d9c-a945-852f80f0eb51" xmlns:ns3="b9355cc9-2d41-4aa9-bfbc-bd016a1e1a01" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f42cd320e09c56919cd7e955403e252" ns2:_="" ns3:_="">
     <xsd:import namespace="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
@@ -3402,25 +3383,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6E40288-91D1-4CD6-86D1-178CC2AEE7EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAAAB53-0ECA-470A-A9D1-4E2A413E8F82}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c4f98862-adfd-4d9c-a945-852f80f0eb51">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED653E30-6791-4489-AE1B-B6DFD5392ED4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3437,4 +3419,22 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAAAB53-0ECA-470A-A9D1-4E2A413E8F82}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6E40288-91D1-4CD6-86D1-178CC2AEE7EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
docs: streamline documentation by removing advanced sections
- Set solver to GLPK in Interface_RDM.xlsx
- Remove Command Options, Pipeline Architecture, and Troubleshooting from Quickstart
- Remove Remote Storage and Customizing Environment from Configuration
- Remove Reproducibility with DVC section from Workflow Overview
- Remove With Options section from RDM Pipeline
- Update PRIM prerequisites to include src/workflow/1_Experiment/ path
- Remove Common DVC Commands, Remote Storage config, and Troubleshooting from DVC Integration
- Remove Contributing Results section and File Formats from Results
- Simplify documentation to focus on core functionality
</commit_message>
<xml_diff>
--- a/src/Interface_RDM.xlsx
+++ b/src/Interface_RDM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\AFR_RDM\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ClimateLeadGroup\Desktop\CLG_repositories\osemosys-rdm\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18ECDC62-1520-4DC9-B4F8-369EBD1541B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CBC0320-271F-494D-9634-6138539A76F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20772" yWindow="2268" windowWidth="17280" windowHeight="8880" tabRatio="727" activeTab="1" xr2:uid="{A38498C0-325E-4D75-9B65-6D8B75ECDFF0}"/>
+    <workbookView xWindow="32670" yWindow="2505" windowWidth="21600" windowHeight="11295" tabRatio="727" activeTab="1" xr2:uid="{A38498C0-325E-4D75-9B65-6D8B75ECDFF0}"/>
   </bookViews>
   <sheets>
     <sheet name="Uncertainty_Table" sheetId="13" r:id="rId1"/>
@@ -733,10 +733,10 @@
     <t>UGA</t>
   </si>
   <si>
-    <t>cplex</t>
-  </si>
-  <si>
     <t>Scenario1</t>
+  </si>
+  <si>
+    <t>glpk</t>
   </si>
 </sst>
 </file>
@@ -1422,7 +1422,7 @@
         <v>142</v>
       </c>
       <c r="D2" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E2" s="15" t="s">
         <v>158</v>
@@ -1467,7 +1467,7 @@
         <v>143</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E3" s="15" t="s">
         <v>158</v>
@@ -1512,7 +1512,7 @@
         <v>156</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>158</v>
@@ -1554,7 +1554,7 @@
         <v>157</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>158</v>
@@ -1596,7 +1596,7 @@
         <v>149</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>158</v>
@@ -1641,7 +1641,7 @@
         <v>150</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>158</v>
@@ -1686,7 +1686,7 @@
         <v>151</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>158</v>
@@ -1731,7 +1731,7 @@
         <v>152</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>158</v>
@@ -1776,7 +1776,7 @@
         <v>154</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>158</v>
@@ -1821,7 +1821,7 @@
         <v>165</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>158</v>
@@ -1866,7 +1866,7 @@
         <v>161</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E12" s="15" t="s">
         <v>158</v>
@@ -1911,7 +1911,7 @@
         <v>168</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E13" s="15" t="s">
         <v>158</v>
@@ -1956,7 +1956,7 @@
         <v>169</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E14" s="15" t="s">
         <v>158</v>
@@ -2001,7 +2001,7 @@
         <v>146</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>158</v>
@@ -2050,7 +2050,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2118,7 +2118,7 @@
         <v>24</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>139</v>
@@ -3167,6 +3167,25 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c4f98862-adfd-4d9c-a945-852f80f0eb51">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BAD73B84EC2FBA4AB6031CFB79C3D0E0" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1d8e6320e34b5f71545ca20c1fb39b21">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c4f98862-adfd-4d9c-a945-852f80f0eb51" xmlns:ns3="b9355cc9-2d41-4aa9-bfbc-bd016a1e1a01" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3f42cd320e09c56919cd7e955403e252" ns2:_="" ns3:_="">
     <xsd:import namespace="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
@@ -3383,26 +3402,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6E40288-91D1-4CD6-86D1-178CC2AEE7EC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c4f98862-adfd-4d9c-a945-852f80f0eb51">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAAAB53-0ECA-470A-A9D1-4E2A413E8F82}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED653E30-6791-4489-AE1B-B6DFD5392ED4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3419,22 +3437,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BAAAAB53-0ECA-470A-A9D1-4E2A413E8F82}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6E40288-91D1-4CD6-86D1-178CC2AEE7EC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c4f98862-adfd-4d9c-a945-852f80f0eb51"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>